<commit_message>
Multiple Sim Verification Added
</commit_message>
<xml_diff>
--- a/Simulations/Tests/z_cutoff_distance.xlsx
+++ b/Simulations/Tests/z_cutoff_distance.xlsx
@@ -5,15 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="zDist_size1000_camKhan" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="zDist_size500_camKhan" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="zDist_size50_camKhan" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="zDist_size200_camKhan" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="zDist_size25_camKhan" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="zDist_size200_camKhan" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="zDist_size50_camKhan" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="zDist_size100_camKhan" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="26">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">test_files_path</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/stb21753492/FiducialTags/Simulations</t>
+    <t xml:space="preserve">/home/paul/FiducialTags/Simulations</t>
   </si>
   <si>
     <t xml:space="preserve">world_file</t>
@@ -64,9 +64,6 @@
     <t xml:space="preserve">vid_pose_file</t>
   </si>
   <si>
-    <t xml:space="preserve">marker_area_file</t>
-  </si>
-  <si>
     <t xml:space="preserve">cameras</t>
   </si>
   <si>
@@ -97,13 +94,13 @@
     <t xml:space="preserve">z_distance_test.txt</t>
   </si>
   <si>
+    <t xml:space="preserve">DICT_4X4_50_s200_id0.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICT_4X4_50_s25_id0.sdf</t>
+  </si>
+  <si>
     <t xml:space="preserve">DICT_4X4_50_s50_id0.sdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICT_4X4_50_s25_id0.sdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICT_4X4_50_s200_id0.sdf</t>
   </si>
   <si>
     <t xml:space="preserve">DICT_4X4_50_s100_id0.sdf</t>
@@ -210,10 +207,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.9"/>
@@ -263,13 +260,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -323,40 +320,32 @@
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>1</v>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -375,13 +364,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -435,40 +424,32 @@
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>1</v>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -487,13 +468,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -516,7 +497,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -547,40 +528,32 @@
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>1</v>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -599,13 +572,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="C77" activeCellId="0" sqref="C77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -628,7 +601,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -659,40 +632,32 @@
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>1</v>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -711,13 +676,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -740,7 +705,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -771,40 +736,32 @@
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>1</v>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -823,13 +780,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -852,7 +809,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -883,40 +840,32 @@
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>1</v>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>